<commit_message>
Renaming and colors refactored.
</commit_message>
<xml_diff>
--- a/chart-component/ui.apps/src/main/content/jcr_root/apps/faizod/components/content/chartcomponent/sample/Sample_Costs_Sales_Profit.xlsx
+++ b/chart-component/ui.apps/src/main/content/jcr_root/apps/faizod/components/content/chartcomponent/sample/Sample_Costs_Sales_Profit.xlsx
@@ -33,13 +33,13 @@
     <t>colors</t>
   </si>
   <si>
-    <t>#000000</t>
+    <t>#4285F4</t>
   </si>
   <si>
-    <t>#ff3300</t>
+    <t>#DB4437</t>
   </si>
   <si>
-    <t>#009900</t>
+    <t>#F4B400</t>
   </si>
 </sst>
 </file>
@@ -381,7 +381,7 @@
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -405,10 +405,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>

</xml_diff>